<commit_message>
modelo com funcoes e restricoes para analise de candidatas. Necessario adicionar a parte binaria do problema
</commit_message>
<xml_diff>
--- a/plan_expansao/plan_geracao/tab_ex.xlsx
+++ b/plan_expansao/plan_geracao/tab_ex.xlsx
@@ -20,11 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Tipo</t>
   </si>
   <si>
+    <t xml:space="preserve">qte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">novas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Capacidade</t>
   </si>
   <si>
@@ -41,6 +47,21 @@
   </si>
   <si>
     <t xml:space="preserve">OeM vari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emissao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limite_comb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mttr</t>
   </si>
   <si>
     <t xml:space="preserve">Óleo</t>
@@ -159,16 +180,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -193,143 +215,290 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="E2" s="1" t="n">
         <v>1294</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="F2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="G2" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>1.42</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="I2" s="1" t="n">
         <v>4.92</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0.2544</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>250000</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>650</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="E3" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="F3" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="G3" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>3.54</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>4.71</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>820</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.4536</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>418</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="E4" s="1" t="n">
         <v>1201</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="F4" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="G4" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>1.23</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="I4" s="1" t="n">
         <v>2.67</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>490</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.02831</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>4525</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="H5" s="1" t="n">
+        <v>10.97</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>5.06</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="N5" s="0" t="n">
         <v>50</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>4525</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>10.97</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>5.06</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="E6" s="1" t="n">
         <v>1411</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="F6" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="n">
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>2.3</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>1920</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="E7" s="1" t="n">
         <v>1323</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="F7" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="n">
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>1.33</v>
       </c>
-      <c r="G7" s="1" t="n">
-        <v>0</v>
+      <c r="I7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>4380</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adição das variaveis inteiras e transformação do problema em MINLP
</commit_message>
<xml_diff>
--- a/plan_expansao/plan_geracao/tab_ex.xlsx
+++ b/plan_expansao/plan_geracao/tab_ex.xlsx
@@ -20,11 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Tipo</t>
   </si>
   <si>
+    <t xml:space="preserve">existentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">novas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Capacidade</t>
   </si>
   <si>
@@ -41,6 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">OeM vari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limite_comb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emissao</t>
   </si>
   <si>
     <t xml:space="preserve">Óleo</t>
@@ -159,16 +174,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -193,142 +208,247 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="E2" s="1" t="n">
         <v>1294</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="F2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="G2" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>1.42</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="I2" s="1" t="n">
         <v>4.92</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>650</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="E3" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="F3" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="G3" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>3.54</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>4.71</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>418</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="E4" s="1" t="n">
         <v>1201</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="F4" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="G4" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>1.23</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="I4" s="1" t="n">
         <v>2.67</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>4525</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>4525</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>10.97</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>5.06</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="E6" s="1" t="n">
         <v>1411</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="F6" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="n">
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>2.3</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="E7" s="1" t="n">
         <v>1323</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="F7" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="n">
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>1.33</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="I7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>